<commit_message>
Last Recheck before form are shared
</commit_message>
<xml_diff>
--- a/data/excel/coordinatorlist.xlsx
+++ b/data/excel/coordinatorlist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE33DAD-B8E3-499C-A22B-A829B91BDF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0586AB-E02A-4CC6-A871-4081A5CADAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{249CFE40-A2DD-4BBF-88EE-17482A72F017}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -94,6 +94,33 @@
   </si>
   <si>
     <t>Priyanshu kulyal</t>
+  </si>
+  <si>
+    <t>Yuvraj Singh</t>
+  </si>
+  <si>
+    <t>Apoorav</t>
+  </si>
+  <si>
+    <t>Table Tennis Co-ordinator</t>
+  </si>
+  <si>
+    <t>Rishabh Singhal</t>
+  </si>
+  <si>
+    <t>Basketball Co-ordinator</t>
+  </si>
+  <si>
+    <t>Gayatri Bisht</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169146090797408256/gay.png?ex=65545725&amp;is=6541e225&amp;hm=ad839237ccb5996c9575a99f2d37193e59b383a6b59c0a4d1aa559ff3983f9ce&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>https://cdn.discordapp.com/attachments/1162451241872412902/1169148446037524590/singal.png?ex=65545957&amp;is=6541e457&amp;hm=cda6b1817a34c9478491dcdeed09606809c069bc99f6163456af737b14982287&amp;</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169148883293708400/dev.png?ex=655459bf&amp;is=6541e4bf&amp;hm=819f02c8367058cc2db46caf3a96aaa9489dded0fe46bbd1315fe78aa3dad846&amp;=&amp;width=380&amp;height=380</t>
   </si>
 </sst>
 </file>
@@ -149,17 +176,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,6 +194,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,114 +512,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C25FC1-1C7C-43BA-9684-6EC797E2D0F8}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.8" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="6">
-        <v>0</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.2" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="9" spans="1:3" ht="16.2" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4"/>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data updated final before launch
</commit_message>
<xml_diff>
--- a/data/excel/coordinatorlist.xlsx
+++ b/data/excel/coordinatorlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0586AB-E02A-4CC6-A871-4081A5CADAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAD2076-CC96-4045-A53D-B509DAE90D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{249CFE40-A2DD-4BBF-88EE-17482A72F017}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -63,15 +63,6 @@
     <t>https://media.discordapp.net/attachments/1162451241872412902/1169130892481019985/organizer.png?ex=655448fe&amp;is=6541d3fe&amp;hm=230f5a32ad5badace3677a959650cb751b71e9a13058e379d1b936af8336301f&amp;=&amp;width=380&amp;height=380</t>
   </si>
   <si>
-    <t>Amit Bisht</t>
-  </si>
-  <si>
-    <t>https://cdn.discordapp.com/attachments/1162451241872412902/1169131684541779978/disipline.png?ex=655449bb&amp;is=6541d4bb&amp;hm=c1d72e460028dd82b3d04417e0276a6fe5078697442fcd78145aa38e44e9692a&amp;</t>
-  </si>
-  <si>
-    <t>Disipline Incharge</t>
-  </si>
-  <si>
     <t>Chess Co-ordinator</t>
   </si>
   <si>
@@ -81,12 +72,6 @@
     <t>https://media.discordapp.net/attachments/1162451241872412902/1169130892166430730/cricketco.png?ex=655448fe&amp;is=6541d3fe&amp;hm=3a703ee136e34d99d6f260a30b0f6708745b832f430b288921530a628ca624e4&amp;=&amp;width=380&amp;height=380</t>
   </si>
   <si>
-    <t>Aron Singh</t>
-  </si>
-  <si>
-    <t>https://media.discordapp.net/attachments/1162451241872412902/1169134082119192597/chessco_1.png?ex=65544bf6&amp;is=6541d6f6&amp;hm=5a442575c9a8ca22f1b67045bbf13d4ee5699372c638b25510f67d88de6642d7&amp;=&amp;width=380&amp;height=380</t>
-  </si>
-  <si>
     <t>Football Co-ordinator</t>
   </si>
   <si>
@@ -99,9 +84,6 @@
     <t>Yuvraj Singh</t>
   </si>
   <si>
-    <t>Apoorav</t>
-  </si>
-  <si>
     <t>Table Tennis Co-ordinator</t>
   </si>
   <si>
@@ -121,6 +103,36 @@
   </si>
   <si>
     <t>https://media.discordapp.net/attachments/1162451241872412902/1169148883293708400/dev.png?ex=655459bf&amp;is=6541e4bf&amp;hm=819f02c8367058cc2db46caf3a96aaa9489dded0fe46bbd1315fe78aa3dad846&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>Apoorav Singh</t>
+  </si>
+  <si>
+    <t>Aaron Singh</t>
+  </si>
+  <si>
+    <t>Nishant Singh Almiya</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169167037944315954/gaya.png?ex=65546aa7&amp;is=6541f5a7&amp;hm=0e0f2e3a2fe807fae36a97e354c315e82f0d0c94fd6d45895cb057099be49491&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>https://cdn.discordapp.com/attachments/1162451241872412902/1169167038174994492/aron.png?ex=65546aa7&amp;is=6541f5a7&amp;hm=33907815ee270399609fb940149c876db334ffa405df6bfc56630205bfe01733&amp;</t>
+  </si>
+  <si>
+    <t>Dheeraj Pathak</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169169287144030238/gaya2.png?ex=65546cc0&amp;is=6541f7c0&amp;hm=284bb7b60d089716f8e4352a23615ad5181aaf2ce6a14eba2ce36d4a5f4e575e&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>Jessica Poona</t>
+  </si>
+  <si>
+    <t>Volleyball Co-ordinator</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169169794222784572/jessie.png?ex=65546d39&amp;is=6541f839&amp;hm=a693765d4cfad95ccf746cf3e61b8fc9c2ee5614f6ab3a44a47905359b2b6786&amp;=&amp;width=380&amp;height=380</t>
   </si>
 </sst>
 </file>
@@ -512,16 +524,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C25FC1-1C7C-43BA-9684-6EC797E2D0F8}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -559,37 +571,37 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.8" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
+      <c r="A5" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
@@ -597,46 +609,68 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.2" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
promise this is final commit
</commit_message>
<xml_diff>
--- a/data/excel/coordinatorlist.xlsx
+++ b/data/excel/coordinatorlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAD2076-CC96-4045-A53D-B509DAE90D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFADC3CE-6A02-4837-88FA-A94844F0162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{249CFE40-A2DD-4BBF-88EE-17482A72F017}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>https://media.discordapp.net/attachments/1162451241872412902/1169169794222784572/jessie.png?ex=65546d39&amp;is=6541f839&amp;hm=a693765d4cfad95ccf746cf3e61b8fc9c2ee5614f6ab3a44a47905359b2b6786&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169227786918043698/land.png?ex=6554a33b&amp;is=65422e3b&amp;hm=1c6018c123d4f2895d36861b46ffc0c6f633e0f943f7f9c33cb747b37625ac04&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169227787199053894/kamlesh_kaniyal.png?ex=6554a33b&amp;is=65422e3b&amp;hm=2340ce8c17d03dee81d7ed6beb788e008fca7d12ffb7a3b53935da73dac4b1ff&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>Kamlesh Kaniyal</t>
+  </si>
+  <si>
+    <t>Rahul Rauleta</t>
   </si>
 </sst>
 </file>
@@ -524,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C25FC1-1C7C-43BA-9684-6EC797E2D0F8}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -673,6 +685,28 @@
         <v>32</v>
       </c>
     </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
final commit for overall data, component.did.mount
</commit_message>
<xml_diff>
--- a/data/excel/coordinatorlist.xlsx
+++ b/data/excel/coordinatorlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFADC3CE-6A02-4837-88FA-A94844F0162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EB776B-8B97-404D-B8F5-0A3C2781F322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{249CFE40-A2DD-4BBF-88EE-17482A72F017}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -145,24 +145,40 @@
   </si>
   <si>
     <t>Rahul Rauleta</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169268557188714537/ADITYA.png?ex=6554c933&amp;is=65425433&amp;hm=a769c7fdb6003443204fc3bb0232188697d1e8a4716e8e336609332737c24ce8&amp;=&amp;width=380&amp;height=380</t>
+  </si>
+  <si>
+    <t>Arm-Wrestling Co-ordinator</t>
+  </si>
+  <si>
+    <t>Aditya tamta</t>
+  </si>
+  <si>
+    <t>Lokesh Joshi</t>
+  </si>
+  <si>
+    <t>Daksh Bisht</t>
+  </si>
+  <si>
+    <t>https://cdn.discordapp.com/attachments/1162451241872412902/1169268556777668698/LOKESH.png?ex=6554c933&amp;is=65425433&amp;hm=381b105654f6d5d82ceee0eacd0b489dfce5e1e909dcde130c912880f5a4e6d1&amp;</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1162451241872412902/1169268558115651614/DASKSH.png?ex=6554c934&amp;is=65425434&amp;hm=b118bb163ba27ed72ed4e81d1caa84d674c5be0b9f38f09df05bd6e8d090cfbc&amp;=&amp;width=380&amp;height=380</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Inherit"/>
     </font>
     <font>
       <sz val="11"/>
@@ -208,18 +224,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,16 +552,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C25FC1-1C7C-43BA-9684-6EC797E2D0F8}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -593,18 +609,18 @@
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -653,58 +669,91 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>